<commit_message>
vista de conflictos funcionando
</commit_message>
<xml_diff>
--- a/controllers/excels/Asistencias a Bases de datos.xlsx
+++ b/controllers/excels/Asistencias a Bases de datos.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>Usuario</t>
   </si>
@@ -92,6 +92,15 @@
   </si>
   <si>
     <t>Coria</t>
+  </si>
+  <si>
+    <t>alumno6@mail.com</t>
+  </si>
+  <si>
+    <t>Quique</t>
+  </si>
+  <si>
+    <t>Quiroga</t>
   </si>
   <si>
     <t>1/2/22</t>
@@ -298,7 +307,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -494,6 +503,44 @@
         <v>15</v>
       </c>
     </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -501,7 +548,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -518,28 +565,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -679,6 +726,41 @@
         <v>15</v>
       </c>
       <c r="K5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="0" t="s">
         <v>15</v>
       </c>
     </row>
@@ -689,7 +771,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -706,31 +788,31 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -747,7 +829,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>15</v>
@@ -823,7 +905,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>15</v>
@@ -882,6 +964,44 @@
         <v>15</v>
       </c>
       <c r="L5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="0" t="s">
         <v>15</v>
       </c>
     </row>
@@ -892,7 +1012,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -909,28 +1029,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1070,6 +1190,41 @@
         <v>15</v>
       </c>
       <c r="K5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="0" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1080,7 +1235,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -1097,34 +1252,34 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1288,6 +1443,47 @@
         <v>15</v>
       </c>
       <c r="M5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="0" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1298,7 +1494,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -1315,28 +1511,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1476,6 +1672,41 @@
         <v>15</v>
       </c>
       <c r="K5" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="0" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1486,7 +1717,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -1503,10 +1734,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1523,7 +1754,7 @@
         <v>15</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1540,7 +1771,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1557,7 +1788,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1574,7 +1805,24 @@
         <v>15</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>15</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>